<commit_message>
changes to collabs table
</commit_message>
<xml_diff>
--- a/data/Field_collabs_MBON_P2P.xlsx
+++ b/data/Field_collabs_MBON_P2P.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20353"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\MBON\GLOBAL_MBON\P2P\P2P_Project\Participants\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enriquemontes/p2p/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1820E5AE-75BA-445A-969F-6E56BF3E1EBE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4386E976-19A5-F747-9BA1-55182AC637A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="25125" windowHeight="16980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10580" yWindow="4000" windowWidth="25120" windowHeight="16980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="P2P_collabs" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="49">
   <si>
     <t>Country</t>
   </si>
@@ -33,126 +33,45 @@
     <t>Affiliation</t>
   </si>
   <si>
-    <t>Universidad del Valle</t>
-  </si>
-  <si>
-    <t>IBIOMAR-CONICET</t>
-  </si>
-  <si>
-    <t>Charles Darwin Foundation</t>
-  </si>
-  <si>
-    <t>Universidad de Guayaquil</t>
-  </si>
-  <si>
-    <t>María Martha Mendez</t>
-  </si>
-  <si>
-    <t>ARGENTINA</t>
-  </si>
-  <si>
-    <t>Juan Pablo Livore</t>
-  </si>
-  <si>
     <t>Lorena Arribas</t>
   </si>
   <si>
-    <t>Universidad Nacional de la Patagonia San Juan Bosco</t>
-  </si>
-  <si>
     <t>José Fernandez Alfaya</t>
   </si>
   <si>
-    <t>universidad Nacional de la Patagonia San Juan Bosco</t>
-  </si>
-  <si>
-    <t>Gonzalo Bravo</t>
-  </si>
-  <si>
-    <t>Maria Fernanda Cardona Gutierrez</t>
-  </si>
-  <si>
-    <t>COLOMBIA</t>
-  </si>
-  <si>
-    <t>Kevin Stiven Mendoza Arcos</t>
-  </si>
-  <si>
     <t>Fabrício Angelo Gabriel</t>
   </si>
   <si>
-    <t>Universidade Federal do Espírito Santo</t>
-  </si>
-  <si>
-    <t>BRAZIL</t>
-  </si>
-  <si>
     <t>Sofia Green</t>
   </si>
   <si>
-    <t>ECUADOR</t>
-  </si>
-  <si>
     <t>Helio Herminio Checon</t>
   </si>
   <si>
-    <t>Universidade de São Paulo</t>
-  </si>
-  <si>
     <t>Paulina Tapia</t>
   </si>
   <si>
-    <t>Universidad de Valparaiso</t>
-  </si>
-  <si>
-    <t>CHILE</t>
-  </si>
-  <si>
     <t>María Jesus Herrera</t>
   </si>
   <si>
     <t>Ricardo Jeldres</t>
   </si>
   <si>
-    <t>Universidad de Concepción</t>
-  </si>
-  <si>
     <t>Viviana Segovia</t>
   </si>
   <si>
-    <t>Universidad Austral</t>
-  </si>
-  <si>
-    <t>Elva Escobar</t>
-  </si>
-  <si>
-    <t>UNAM</t>
-  </si>
-  <si>
     <t>Ma del Socorro García Madrigal</t>
   </si>
   <si>
-    <t>La Universidad del Mar, campus Puerto Ángel,</t>
-  </si>
-  <si>
     <t>Raul Zambrano</t>
   </si>
   <si>
-    <t>BIOELITE</t>
-  </si>
-  <si>
     <t>Cristian Campuzano</t>
   </si>
   <si>
     <t>Martha Montero</t>
   </si>
   <si>
-    <t>Andrea Torres</t>
-  </si>
-  <si>
-    <t>Universidad de Especialidades Espíritu Santo</t>
-  </si>
-  <si>
     <t>Michael Martillo</t>
   </si>
   <si>
@@ -165,9 +84,6 @@
     <t>Zehila Zambrano</t>
   </si>
   <si>
-    <t>Universidad Península de Santa Elena</t>
-  </si>
-  <si>
     <t>Jefferson Arcos</t>
   </si>
   <si>
@@ -177,7 +93,85 @@
     <t>María Muciño</t>
   </si>
   <si>
-    <t>MEXICO</t>
+    <t>[María Martha Mendez](https://oceanexpert.org/expert/33363)</t>
+  </si>
+  <si>
+    <t>[IBIOMAR/CONICET](https://www.larbim.com.ar/)</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>[Juan Pablo Livore](https://oceanexpert.org/expert/29793)</t>
+  </si>
+  <si>
+    <t>[Gonzalo Bravo](https://oceanexpert.org/expert/39346)</t>
+  </si>
+  <si>
+    <t>[Universidad Nacional de la Patagonia San Juan Bosco](http://www.unp.edu.ar/)</t>
+  </si>
+  <si>
+    <t>[Maria F. Cardona Gutierrez](https://oceanexpert.org/expert/35044)</t>
+  </si>
+  <si>
+    <t>Kevin S. Mendoza Arcos</t>
+  </si>
+  <si>
+    <t>[U. del Valle](https://lithos.correounivalle.edu.co/)</t>
+  </si>
+  <si>
+    <t>Colombia</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Ecuador</t>
+  </si>
+  <si>
+    <t>Chile</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>[Charles Darwin F.](https://www.darwinfoundation.org/en/)</t>
+  </si>
+  <si>
+    <t>[RIEAE - U. Guayaquil](https://www.facebook.com/RED-RIEAE-107397151044316)</t>
+  </si>
+  <si>
+    <t>[Universidad de Guayaquil](http://www.ug.edu.ec/)</t>
+  </si>
+  <si>
+    <t>[UPSE](https://www.upse.edu.ec/)</t>
+  </si>
+  <si>
+    <t>[UEES](https://www.uees.edu.ec/)</t>
+  </si>
+  <si>
+    <t>[UNAM](https://www.bdmy.org.mx/)</t>
+  </si>
+  <si>
+    <t>[UMAR](http://www.umar.mx/)</t>
+  </si>
+  <si>
+    <t>[Universidad Austral](https://www.austral.edu.ar/en/)</t>
+  </si>
+  <si>
+    <t>[U. Concepcion](http://www6.udec.cl/pexterno/)</t>
+  </si>
+  <si>
+    <t>[Universidad de Valparaiso](https://www.uv.cl/)</t>
+  </si>
+  <si>
+    <t>[USP](https://www5.usp.br/)</t>
+  </si>
+  <si>
+    <t>[Bentos - UFES](http://bentos.ufes.br/)</t>
+  </si>
+  <si>
+    <t>[Andrea Torres](https://oceanexpert.org/expert/29554)</t>
   </si>
 </sst>
 </file>
@@ -563,22 +557,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.1640625" customWidth="1"/>
+    <col min="2" max="2" width="45.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -587,290 +581,279 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>36</v>
       </c>
       <c r="B19" t="s">
         <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
         <v>37</v>
       </c>
       <c r="C20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" t="s">
         <v>39</v>
       </c>
-      <c r="B21" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C24" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" t="s">
-        <v>5</v>
-      </c>
       <c r="C25" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C26" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>47</v>
-      </c>
-      <c r="B27" t="s">
-        <v>46</v>
-      </c>
-      <c r="C27" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added {target="_blank"} to URL in Members, Events, others
</commit_message>
<xml_diff>
--- a/data/Field_collabs_MBON_P2P.xlsx
+++ b/data/Field_collabs_MBON_P2P.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11213"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enriquemontes/p2p/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4386E976-19A5-F747-9BA1-55182AC637A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31BF914-6253-644D-B719-66F5C105A49B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10580" yWindow="4000" windowWidth="25120" windowHeight="16980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -93,33 +93,12 @@
     <t>María Muciño</t>
   </si>
   <si>
-    <t>[María Martha Mendez](https://oceanexpert.org/expert/33363)</t>
-  </si>
-  <si>
-    <t>[IBIOMAR/CONICET](https://www.larbim.com.ar/)</t>
-  </si>
-  <si>
     <t>Argentina</t>
   </si>
   <si>
-    <t>[Juan Pablo Livore](https://oceanexpert.org/expert/29793)</t>
-  </si>
-  <si>
-    <t>[Gonzalo Bravo](https://oceanexpert.org/expert/39346)</t>
-  </si>
-  <si>
-    <t>[Universidad Nacional de la Patagonia San Juan Bosco](http://www.unp.edu.ar/)</t>
-  </si>
-  <si>
-    <t>[Maria F. Cardona Gutierrez](https://oceanexpert.org/expert/35044)</t>
-  </si>
-  <si>
     <t>Kevin S. Mendoza Arcos</t>
   </si>
   <si>
-    <t>[U. del Valle](https://lithos.correounivalle.edu.co/)</t>
-  </si>
-  <si>
     <t>Colombia</t>
   </si>
   <si>
@@ -135,43 +114,64 @@
     <t>Mexico</t>
   </si>
   <si>
-    <t>[Charles Darwin F.](https://www.darwinfoundation.org/en/)</t>
-  </si>
-  <si>
-    <t>[RIEAE - U. Guayaquil](https://www.facebook.com/RED-RIEAE-107397151044316)</t>
-  </si>
-  <si>
-    <t>[Universidad de Guayaquil](http://www.ug.edu.ec/)</t>
-  </si>
-  <si>
-    <t>[UPSE](https://www.upse.edu.ec/)</t>
-  </si>
-  <si>
-    <t>[UEES](https://www.uees.edu.ec/)</t>
-  </si>
-  <si>
-    <t>[UNAM](https://www.bdmy.org.mx/)</t>
-  </si>
-  <si>
-    <t>[UMAR](http://www.umar.mx/)</t>
-  </si>
-  <si>
-    <t>[Universidad Austral](https://www.austral.edu.ar/en/)</t>
-  </si>
-  <si>
-    <t>[U. Concepcion](http://www6.udec.cl/pexterno/)</t>
-  </si>
-  <si>
-    <t>[Universidad de Valparaiso](https://www.uv.cl/)</t>
-  </si>
-  <si>
-    <t>[USP](https://www5.usp.br/)</t>
-  </si>
-  <si>
-    <t>[Bentos - UFES](http://bentos.ufes.br/)</t>
-  </si>
-  <si>
-    <t>[Andrea Torres](https://oceanexpert.org/expert/29554)</t>
+    <t>[María Martha Mendez](https://oceanexpert.org/expert/33363){target="_blank"}</t>
+  </si>
+  <si>
+    <t>[Juan Pablo Livore](https://oceanexpert.org/expert/29793){target="_blank"}</t>
+  </si>
+  <si>
+    <t>[Gonzalo Bravo](https://oceanexpert.org/expert/39346){target="_blank"}</t>
+  </si>
+  <si>
+    <t>[Maria F. Cardona Gutierrez](https://oceanexpert.org/expert/35044){target="_blank"}</t>
+  </si>
+  <si>
+    <t>[Andrea Torres](https://oceanexpert.org/expert/29554){target="_blank"}</t>
+  </si>
+  <si>
+    <t>[IBIOMAR/CONICET](https://www.larbim.com.ar/){target="_blank"}</t>
+  </si>
+  <si>
+    <t>[Universidad Nacional de la Patagonia San Juan Bosco](http://www.unp.edu.ar/){target="_blank"}</t>
+  </si>
+  <si>
+    <t>[U. del Valle](https://lithos.correounivalle.edu.co/){target="_blank"}</t>
+  </si>
+  <si>
+    <t>[Bentos - UFES](http://bentos.ufes.br/){target="_blank"}</t>
+  </si>
+  <si>
+    <t>[USP](https://www5.usp.br/){target="_blank"}</t>
+  </si>
+  <si>
+    <t>[Universidad de Valparaiso](https://www.uv.cl/){target="_blank"}</t>
+  </si>
+  <si>
+    <t>[U. Concepcion](http://www6.udec.cl/pexterno/){target="_blank"}</t>
+  </si>
+  <si>
+    <t>[Universidad Austral](https://www.austral.edu.ar/en/){target="_blank"}</t>
+  </si>
+  <si>
+    <t>[UMAR](http://www.umar.mx/){target="_blank"}</t>
+  </si>
+  <si>
+    <t>[UNAM](https://www.bdmy.org.mx/){target="_blank"}</t>
+  </si>
+  <si>
+    <t>[Charles Darwin F.](https://www.darwinfoundation.org/en/){target="_blank"}</t>
+  </si>
+  <si>
+    <t>[RIEAE - U. Guayaquil](https://www.facebook.com/RED-RIEAE-107397151044316){target="_blank"}</t>
+  </si>
+  <si>
+    <t>[UEES](https://www.uees.edu.ec/){target="_blank"}</t>
+  </si>
+  <si>
+    <t>[Universidad de Guayaquil](http://www.ug.edu.ec/){target="_blank"}</t>
+  </si>
+  <si>
+    <t>[UPSE](https://www.upse.edu.ec/){target="_blank"}</t>
   </si>
 </sst>
 </file>
@@ -560,7 +560,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -583,24 +583,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
         <v>22</v>
-      </c>
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -608,10 +608,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -619,43 +619,43 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -663,10 +663,10 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -674,10 +674,10 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -685,10 +685,10 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -696,10 +696,10 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -707,10 +707,10 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -718,10 +718,10 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -732,7 +732,7 @@
         <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -740,10 +740,10 @@
         <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -751,10 +751,10 @@
         <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -762,10 +762,10 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -773,10 +773,10 @@
         <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C19" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -784,21 +784,21 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C20" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C21" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -806,10 +806,10 @@
         <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C22" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -817,10 +817,10 @@
         <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C23" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -828,10 +828,10 @@
         <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C24" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -839,10 +839,10 @@
         <v>18</v>
       </c>
       <c r="B25" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="C25" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -850,10 +850,10 @@
         <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="C26" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>